<commit_message>
Seeting up IMAGE-ODYM Translator for FutureDemand, FinalProducts_2015 and Material Content (MC)
</commit_message>
<xml_diff>
--- a/Data/3_LT_RECC_ProductLifetime_appliances_V1.0.xlsx
+++ b/Data/3_LT_RECC_ProductLifetime_appliances_V1.0.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="210">
   <si>
     <t>id</t>
   </si>
@@ -341,69 +341,6 @@
     <t>Created by IEDC_tools v0.4.0</t>
   </si>
   <si>
-    <t>aspect 1 : commodity</t>
-  </si>
-  <si>
-    <t>aspect 2 : process</t>
-  </si>
-  <si>
-    <t>aspect 3 : region</t>
-  </si>
-  <si>
-    <t>aspect 4 : age-cohort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspect 5 : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspect 6 : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspect 7 : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspect 8 : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspect 9 : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspect 10 : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspect 11 : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspect 12 : </t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>unitcode</t>
-  </si>
-  <si>
-    <t>unitcode1</t>
-  </si>
-  <si>
-    <t>stats_array_1</t>
-  </si>
-  <si>
-    <t>stats_array_2</t>
-  </si>
-  <si>
-    <t>stats_array_3</t>
-  </si>
-  <si>
-    <t>stats_array_4</t>
-  </si>
-  <si>
-    <t>Internal Combustion Engine (ICE)</t>
-  </si>
-  <si>
-    <t>use phase</t>
-  </si>
-  <si>
     <t>yr</t>
   </si>
   <si>
@@ -416,18 +353,6 @@
     <t>Avg. lifetime calculated from Weibull distr. parameters, scale = 1/lambda and shape = k.</t>
   </si>
   <si>
-    <t>Hybrid Electric Vehicles (HEV)</t>
-  </si>
-  <si>
-    <t>Plugin Hybrid Electric Vehicles (PHEV)</t>
-  </si>
-  <si>
-    <t>Battery Electric Vehicles (BEV)</t>
-  </si>
-  <si>
-    <t>Fuel Cell Vehicles (FCV)</t>
-  </si>
-  <si>
     <t>Fan</t>
   </si>
   <si>
@@ -617,9 +542,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Unit of mean lifetime</t>
-  </si>
-  <si>
     <t># Aspects_Meaning: Describe meaning of each aspect</t>
   </si>
   <si>
@@ -653,7 +575,82 @@
     <t>2a33b48a-aed8-11e9-a2a3-2a2ae2dbcce4</t>
   </si>
   <si>
-    <t>Lifetimes of appliances in use phase, for RECC project, taken from DEETMAN et a. 2018</t>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Stats_array_string</t>
+  </si>
+  <si>
+    <t>use phase, Fan</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=1.3;</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>use phase, Air-cooler</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=2;</t>
+  </si>
+  <si>
+    <t>use phase, Air-conditioning</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=2.8;</t>
+  </si>
+  <si>
+    <t>use phase, Refridgerator</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=2.2;</t>
+  </si>
+  <si>
+    <t>use phase, Microwave</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=0.8;</t>
+  </si>
+  <si>
+    <t>use phase, Washing Machine</t>
+  </si>
+  <si>
+    <t>use phase, Tumble dryer</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=2.6;</t>
+  </si>
+  <si>
+    <t>use phase, Dish washer</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=1.6;</t>
+  </si>
+  <si>
+    <t>use phase, Television</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=2.1;</t>
+  </si>
+  <si>
+    <t>use phase, VCR/DVD player</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=1.7;</t>
+  </si>
+  <si>
+    <t>use phase, PC &amp; Laptop computers</t>
+  </si>
+  <si>
+    <t>8;'shape'=Value;'scale'=1.5;</t>
+  </si>
+  <si>
+    <t>use phase, Other small appliances</t>
+  </si>
+  <si>
+    <t>Lifetimes of appliances in use phase, for RECC project, taken from DEETMAN et al. (2018)</t>
   </si>
 </sst>
 </file>
@@ -734,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,12 +758,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -791,34 +804,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table11" displayName="Table11" ref="A1:Y18" totalsRowShown="0">
-  <autoFilter ref="A1:Y18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table11" displayName="Table11" ref="A2:Y18" headerRowCount="0" totalsRowShown="0" headerRowDxfId="0">
   <tableColumns count="25">
-    <tableColumn id="1" name="id"/>
-    <tableColumn id="2" name="dataset_name"/>
-    <tableColumn id="3" name="aspect 1 : commodity"/>
-    <tableColumn id="4" name="aspect 2 : process"/>
-    <tableColumn id="5" name="aspect 3 : region"/>
-    <tableColumn id="6" name="aspect 4 : age-cohort"/>
-    <tableColumn id="7" name="aspect 5 : "/>
-    <tableColumn id="8" name="aspect 6 : "/>
-    <tableColumn id="9" name="aspect 7 : "/>
-    <tableColumn id="10" name="aspect 8 : "/>
-    <tableColumn id="11" name="aspect 9 : "/>
-    <tableColumn id="12" name="aspect 10 : "/>
-    <tableColumn id="13" name="aspect 11 : "/>
-    <tableColumn id="14" name="aspect 12 : "/>
-    <tableColumn id="15" name="value"/>
-    <tableColumn id="16" name="unitcode"/>
-    <tableColumn id="17" name="unitcode1"/>
-    <tableColumn id="18" name="stats_array_1"/>
-    <tableColumn id="19" name="stats_array_2"/>
-    <tableColumn id="20" name="stats_array_3"/>
-    <tableColumn id="21" name="stats_array_4"/>
-    <tableColumn id="22" name="comment"/>
-    <tableColumn id="23" name="reserve1"/>
-    <tableColumn id="24" name="reserve2"/>
-    <tableColumn id="25" name="reserve3"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
+    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="9" name="Column9"/>
+    <tableColumn id="10" name="Column10"/>
+    <tableColumn id="11" name="Column11"/>
+    <tableColumn id="12" name="Column12"/>
+    <tableColumn id="13" name="Column13"/>
+    <tableColumn id="14" name="Column14"/>
+    <tableColumn id="15" name="Column15"/>
+    <tableColumn id="16" name="Column16"/>
+    <tableColumn id="17" name="Column17"/>
+    <tableColumn id="18" name="Column18"/>
+    <tableColumn id="19" name="Column19"/>
+    <tableColumn id="20" name="Column20"/>
+    <tableColumn id="21" name="Column21"/>
+    <tableColumn id="22" name="Column22"/>
+    <tableColumn id="23" name="Column23"/>
+    <tableColumn id="24" name="Column24"/>
+    <tableColumn id="25" name="Column25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1111,7 +1123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A29" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1594,18 +1606,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.21875" customWidth="1"/>
     <col min="3" max="3" width="33.77734375" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="30.21875" customWidth="1"/>
     <col min="7" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="14" width="13.77734375" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" customWidth="1"/>
@@ -1616,784 +1630,538 @@
     <col min="23" max="25" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="26">
+        <v>9.4</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="26">
+        <v>13.5</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="26">
+        <v>12.3</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="26">
+        <v>16.5</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="26">
+        <v>14.7</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="26">
+        <v>13.9</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="O7" s="23">
+        <v>8.6816211826261895</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R7" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T7" s="23">
+        <v>9.4</v>
+      </c>
+      <c r="U7" s="23">
+        <v>1.3</v>
+      </c>
+      <c r="V7" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="26">
+        <v>16.5</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="O8" s="23">
+        <v>11.964063493612199</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q8" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T8" s="23">
+        <v>13.5</v>
+      </c>
+      <c r="U8" s="23">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="V8" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="26">
+        <v>13.1</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F9" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="O9" s="23">
+        <v>10.952546728525</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q9" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="E1" t="s">
+      <c r="R9" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="F1" t="s">
+      <c r="T9" s="23">
+        <v>12.3</v>
+      </c>
+      <c r="U9" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="V9" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="G1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L1" t="s">
-        <v>115</v>
-      </c>
-      <c r="M1" t="s">
-        <v>116</v>
-      </c>
-      <c r="N1" t="s">
-        <v>117</v>
-      </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="10" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="P1" t="s">
+      <c r="B10" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" s="26">
+        <v>12</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="O10" s="23">
+        <v>14.612808547428401</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q10" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R10" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T10" s="23">
+        <v>16.5</v>
+      </c>
+      <c r="U10" s="23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V10" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="B11" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="26">
+        <v>10.5</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="O11" s="23">
+        <v>16.6551455158944</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q11" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R11" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T11" s="23">
+        <v>14.7</v>
+      </c>
+      <c r="U11" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="V11" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B12" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" s="26">
+        <v>5.2</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="O12" s="23">
+        <v>12.3101841702579</v>
+      </c>
+      <c r="P12" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q12" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R12" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T12" s="23">
+        <v>13.9</v>
+      </c>
+      <c r="U12" s="23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V12" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="S1" t="s">
-        <v>122</v>
-      </c>
-      <c r="T1" t="s">
-        <v>123</v>
-      </c>
-      <c r="U1" t="s">
-        <v>124</v>
-      </c>
-      <c r="V1" t="s">
-        <v>37</v>
-      </c>
-      <c r="W1" t="s">
-        <v>100</v>
-      </c>
-      <c r="X1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>32159</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2">
-        <v>9.1414223077736896</v>
-      </c>
-      <c r="P2" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>128</v>
-      </c>
-      <c r="R2" t="s">
-        <v>129</v>
-      </c>
-      <c r="T2">
-        <v>10.3</v>
-      </c>
-      <c r="U2">
-        <v>1.89</v>
-      </c>
-      <c r="V2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>32160</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3">
-        <v>9.1414223077736896</v>
-      </c>
-      <c r="P3" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>128</v>
-      </c>
-      <c r="R3" t="s">
-        <v>129</v>
-      </c>
-      <c r="T3">
-        <v>10.3</v>
-      </c>
-      <c r="U3">
-        <v>1.89</v>
-      </c>
-      <c r="V3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>32161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4">
-        <v>9.1414223077736896</v>
-      </c>
-      <c r="P4" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>128</v>
-      </c>
-      <c r="R4" t="s">
-        <v>129</v>
-      </c>
-      <c r="T4">
-        <v>10.3</v>
-      </c>
-      <c r="U4">
-        <v>1.89</v>
-      </c>
-      <c r="V4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>32162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5">
-        <v>9.1414223077736896</v>
-      </c>
-      <c r="P5" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>128</v>
-      </c>
-      <c r="R5" t="s">
-        <v>129</v>
-      </c>
-      <c r="T5">
-        <v>10.3</v>
-      </c>
-      <c r="U5">
-        <v>1.89</v>
-      </c>
-      <c r="V5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>32163</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6">
-        <v>9.1414223077736896</v>
-      </c>
-      <c r="P6" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>128</v>
-      </c>
-      <c r="R6" t="s">
-        <v>129</v>
-      </c>
-      <c r="T6">
-        <v>10.3</v>
-      </c>
-      <c r="U6">
-        <v>1.89</v>
-      </c>
-      <c r="V6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>32164</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7">
-        <v>8.6816211826261895</v>
-      </c>
-      <c r="P7" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>128</v>
-      </c>
-      <c r="R7" t="s">
-        <v>129</v>
-      </c>
-      <c r="T7">
-        <v>9.4</v>
-      </c>
-      <c r="U7">
-        <v>1.3</v>
-      </c>
-      <c r="V7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>32165</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8">
-        <v>11.964063493612199</v>
-      </c>
-      <c r="P8" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>128</v>
-      </c>
-      <c r="R8" t="s">
-        <v>129</v>
-      </c>
-      <c r="T8">
-        <v>13.5</v>
-      </c>
-      <c r="U8">
-        <v>2</v>
-      </c>
-      <c r="V8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>32166</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9">
-        <v>10.952546728525</v>
-      </c>
-      <c r="P9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>128</v>
-      </c>
-      <c r="R9" t="s">
-        <v>129</v>
-      </c>
-      <c r="T9">
-        <v>12.3</v>
-      </c>
-      <c r="U9">
-        <v>2.8</v>
-      </c>
-      <c r="V9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>32167</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10">
-        <v>14.612808547428401</v>
-      </c>
-      <c r="P10" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>128</v>
-      </c>
-      <c r="R10" t="s">
-        <v>129</v>
-      </c>
-      <c r="T10">
+      <c r="B13" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="26">
+        <v>4</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="O13" s="23">
+        <v>14.655472173093001</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q13" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R13" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T13" s="23">
         <v>16.5</v>
       </c>
-      <c r="U10">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="V10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>32168</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-      <c r="O11">
-        <v>16.6551455158944</v>
-      </c>
-      <c r="P11" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>128</v>
-      </c>
-      <c r="R11" t="s">
-        <v>129</v>
-      </c>
-      <c r="T11">
-        <v>14.7</v>
-      </c>
-      <c r="U11">
-        <v>0.8</v>
-      </c>
-      <c r="V11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>32169</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12">
-        <v>12.3101841702579</v>
-      </c>
-      <c r="P12" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>128</v>
-      </c>
-      <c r="R12" t="s">
-        <v>129</v>
-      </c>
-      <c r="T12">
-        <v>13.9</v>
-      </c>
-      <c r="U12">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="V12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>32170</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13">
-        <v>14.655472173093001</v>
-      </c>
-      <c r="P13" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>128</v>
-      </c>
-      <c r="R13" t="s">
-        <v>129</v>
-      </c>
-      <c r="T13">
-        <v>16.5</v>
-      </c>
-      <c r="U13">
+      <c r="U13" s="23">
         <v>2.6</v>
       </c>
-      <c r="V13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>32171</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D14" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="O14">
+      <c r="V13" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O14" s="23">
         <v>11.7451230687414</v>
       </c>
-      <c r="P14" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>128</v>
-      </c>
-      <c r="R14" t="s">
-        <v>129</v>
-      </c>
-      <c r="T14">
+      <c r="P14" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q14" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R14" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T14" s="23">
         <v>13.1</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="23">
         <v>1.6</v>
       </c>
-      <c r="V14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>32172</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
-      <c r="O15">
+      <c r="V14" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O15" s="23">
         <v>10.6283233670864</v>
       </c>
-      <c r="P15" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>128</v>
-      </c>
-      <c r="R15" t="s">
-        <v>129</v>
-      </c>
-      <c r="T15">
+      <c r="P15" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q15" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R15" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T15" s="23">
         <v>12</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="23">
         <v>2.1</v>
       </c>
-      <c r="V15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>32173</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16">
+      <c r="V15" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O16" s="23">
         <v>9.3685672762428993</v>
       </c>
-      <c r="P16" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>128</v>
-      </c>
-      <c r="R16" t="s">
-        <v>129</v>
-      </c>
-      <c r="T16">
+      <c r="P16" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q16" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R16" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T16" s="23">
         <v>10.5</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="23">
         <v>1.7</v>
       </c>
-      <c r="V16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>32174</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D17" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17">
+      <c r="V16" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="15:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O17" s="23">
         <v>4.6942755233448503</v>
       </c>
-      <c r="P17" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>128</v>
-      </c>
-      <c r="R17" t="s">
-        <v>129</v>
-      </c>
-      <c r="T17">
+      <c r="P17" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q17" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R17" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T17" s="23">
         <v>5.2</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="23">
         <v>1.5</v>
       </c>
-      <c r="V17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>32175</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>26</v>
-      </c>
-      <c r="O18">
+      <c r="V17" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="15:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O18" s="23">
         <v>3.6109811718037399</v>
       </c>
-      <c r="P18" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>128</v>
-      </c>
-      <c r="R18" t="s">
-        <v>129</v>
-      </c>
-      <c r="T18">
+      <c r="P18" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q18" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="R18" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="T18" s="23">
         <v>4</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="23">
         <v>1.5</v>
       </c>
-      <c r="V18" t="s">
-        <v>130</v>
-      </c>
-    </row>
+      <c r="V18" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="15:22" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="15:22" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2403,7 +2171,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2414,18 +2182,18 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="4" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -2435,20 +2203,20 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="6" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -2458,20 +2226,20 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="6" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2481,20 +2249,20 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -2504,20 +2272,20 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -2527,20 +2295,20 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -2550,20 +2318,20 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -2573,20 +2341,20 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2596,20 +2364,20 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2619,20 +2387,20 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2642,7 +2410,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="B11" s="10">
         <v>43671</v>
@@ -2650,12 +2418,12 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2665,7 +2433,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="B12" s="10">
         <v>43671</v>
@@ -2673,12 +2441,12 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2688,20 +2456,20 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2711,20 +2479,20 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2734,20 +2502,20 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2757,7 +2525,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -2774,7 +2542,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -2791,7 +2559,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -2808,7 +2576,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -2825,7 +2593,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -2842,24 +2610,24 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="D21" s="14">
         <v>480</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2869,19 +2637,19 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
@@ -2894,24 +2662,24 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="16" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2921,24 +2689,24 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="18" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2948,24 +2716,24 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="18" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2977,18 +2745,18 @@
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="17" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -3002,7 +2770,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="2"/>
@@ -3019,7 +2787,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="2"/>
@@ -3036,7 +2804,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="2"/>
@@ -3053,7 +2821,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="3" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="2"/>

</xml_diff>

<commit_message>
All input files are read now
</commit_message>
<xml_diff>
--- a/Data/3_LT_RECC_ProductLifetime_appliances_V1.0.xlsx
+++ b/Data/3_LT_RECC_ProductLifetime_appliances_V1.0.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11640" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset description" sheetId="2" r:id="rId1"/>
-    <sheet name="Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Values_Master" sheetId="3" r:id="rId2"/>
     <sheet name="Cover" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="198">
   <si>
     <t>id</t>
   </si>
@@ -524,9 +524,6 @@
     <t>Products_m3</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -536,21 +533,12 @@
     <t xml:space="preserve"># Aspects: Specify aspects in order of appearance in data table. </t>
   </si>
   <si>
-    <t>Process</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
     <t># Aspects_Meaning: Describe meaning of each aspect</t>
   </si>
   <si>
-    <t>SSP_Regions_32</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
     <t>Stats_Array_String</t>
   </si>
   <si>
@@ -575,82 +563,58 @@
     <t>2a33b48a-aed8-11e9-a2a3-2a2ae2dbcce4</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>Stats_array_string</t>
   </si>
   <si>
-    <t>use phase, Fan</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=1.3;</t>
   </si>
   <si>
-    <t>global</t>
-  </si>
-  <si>
-    <t>use phase, Air-cooler</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=2;</t>
   </si>
   <si>
-    <t>use phase, Air-conditioning</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=2.8;</t>
   </si>
   <si>
-    <t>use phase, Refridgerator</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=2.2;</t>
   </si>
   <si>
-    <t>use phase, Microwave</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=0.8;</t>
   </si>
   <si>
-    <t>use phase, Washing Machine</t>
-  </si>
-  <si>
-    <t>use phase, Tumble dryer</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=2.6;</t>
   </si>
   <si>
-    <t>use phase, Dish washer</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=1.6;</t>
   </si>
   <si>
-    <t>use phase, Television</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=2.1;</t>
   </si>
   <si>
-    <t>use phase, VCR/DVD player</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=1.7;</t>
   </si>
   <si>
-    <t>use phase, PC &amp; Laptop computers</t>
-  </si>
-  <si>
     <t>8;'shape'=Value;'scale'=1.5;</t>
   </si>
   <si>
-    <t>use phase, Other small appliances</t>
-  </si>
-  <si>
     <t>Lifetimes of appliances in use phase, for RECC project, taken from DEETMAN et al. (2018)</t>
+  </si>
+  <si>
+    <t>SSP_Regions_1</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>wOrld o</t>
+  </si>
+  <si>
+    <t>good g</t>
+  </si>
+  <si>
+    <t>Unit of mean lifetime</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -759,18 +723,106 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -804,16 +856,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table11" displayName="Table11" ref="A2:Y18" headerRowCount="0" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table11" displayName="Table11" ref="A2:Y18" headerRowCount="0" totalsRowShown="0" headerRowDxfId="8">
   <tableColumns count="25">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="1" name="Column1" dataDxfId="7"/>
+    <tableColumn id="2" name="Column2" dataDxfId="6"/>
+    <tableColumn id="3" name="Column3" dataDxfId="5"/>
+    <tableColumn id="4" name="Column4" dataDxfId="4"/>
+    <tableColumn id="5" name="Column5" dataDxfId="3"/>
+    <tableColumn id="6" name="Column6" dataDxfId="2"/>
+    <tableColumn id="7" name="Column7" dataDxfId="1"/>
+    <tableColumn id="8" name="Column8" dataDxfId="0"/>
     <tableColumn id="9" name="Column9"/>
     <tableColumn id="10" name="Column10"/>
     <tableColumn id="11" name="Column11"/>
@@ -1608,19 +1660,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.21875" customWidth="1"/>
-    <col min="7" max="11" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" customWidth="1"/>
+    <col min="4" max="4" width="33.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="30.21875" customWidth="1"/>
+    <col min="8" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="14" width="13.77734375" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" customWidth="1"/>
     <col min="16" max="16" width="12.109375" customWidth="1"/>
@@ -1630,533 +1683,503 @@
     <col min="23" max="25" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>139</v>
-      </c>
       <c r="C1" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="F1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="25">
+        <v>9.4</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="25">
+        <v>13.5</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="25">
+        <v>12.3</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="25">
+        <v>16.5</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="25">
+        <v>14.7</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="25" t="s">
+    </row>
+    <row r="7" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="25">
+        <v>13.9</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="O7" s="22">
+        <v>8.6816211826261895</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R7" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T7" s="22">
+        <v>9.4</v>
+      </c>
+      <c r="U7" s="22">
+        <v>1.3</v>
+      </c>
+      <c r="V7" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="25">
+        <v>16.5</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="O8" s="22">
+        <v>11.964063493612199</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R8" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T8" s="22">
+        <v>13.5</v>
+      </c>
+      <c r="U8" s="22">
+        <v>2</v>
+      </c>
+      <c r="V8" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="25">
+        <v>13.1</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="O9" s="22">
+        <v>10.952546728525</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q9" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R9" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T9" s="22">
+        <v>12.3</v>
+      </c>
+      <c r="U9" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="V9" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="25">
+        <v>12</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="26">
-        <v>9.4</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="O10" s="22">
+        <v>14.612808547428401</v>
+      </c>
+      <c r="P10" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="Q10" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R10" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T10" s="22">
+        <v>16.5</v>
+      </c>
+      <c r="U10" s="22">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V10" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="25">
+        <v>10.5</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="26">
-        <v>13.5</v>
-      </c>
-      <c r="E3" s="24" t="s">
+      <c r="O11" s="22">
+        <v>16.6551455158944</v>
+      </c>
+      <c r="P11" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="Q11" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R11" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T11" s="22">
+        <v>14.7</v>
+      </c>
+      <c r="U11" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="V11" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="25">
+        <v>5.2</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" s="26">
-        <v>12.3</v>
-      </c>
-      <c r="E4" s="24" t="s">
+      <c r="O12" s="22">
+        <v>12.3101841702579</v>
+      </c>
+      <c r="P12" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="25" t="s">
+      <c r="Q12" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R12" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T12" s="22">
+        <v>13.9</v>
+      </c>
+      <c r="U12" s="22">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V12" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="26">
+      <c r="B13" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="25">
+        <v>4</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="O13" s="22">
+        <v>14.655472173093001</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q13" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R13" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T13" s="22">
         <v>16.5</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="U13" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="V13" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="O14" s="22">
+        <v>11.7451230687414</v>
+      </c>
+      <c r="P14" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="25" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D6" s="26">
-        <v>14.7</v>
-      </c>
-      <c r="E6" s="24" t="s">
+      <c r="Q14" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R14" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T14" s="22">
+        <v>13.1</v>
+      </c>
+      <c r="U14" s="22">
+        <v>1.6</v>
+      </c>
+      <c r="V14" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="O15" s="22">
+        <v>10.6283233670864</v>
+      </c>
+      <c r="P15" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D7" s="26">
-        <v>13.9</v>
-      </c>
-      <c r="E7" s="24" t="s">
+      <c r="Q15" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R15" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T15" s="22">
+        <v>12</v>
+      </c>
+      <c r="U15" s="22">
+        <v>2.1</v>
+      </c>
+      <c r="V15" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="O16" s="22">
+        <v>9.3685672762428993</v>
+      </c>
+      <c r="P16" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="O7" s="23">
-        <v>8.6816211826261895</v>
-      </c>
-      <c r="P7" s="23" t="s">
+      <c r="Q16" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="R16" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T16" s="22">
+        <v>10.5</v>
+      </c>
+      <c r="U16" s="22">
+        <v>1.7</v>
+      </c>
+      <c r="V16" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="O17" s="22">
+        <v>4.6942755233448503</v>
+      </c>
+      <c r="P17" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="Q7" s="23" t="s">
+      <c r="Q17" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="R17" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="T7" s="23">
-        <v>9.4</v>
-      </c>
-      <c r="U7" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="V7" s="23" t="s">
+      <c r="T17" s="22">
+        <v>5.2</v>
+      </c>
+      <c r="U17" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="V17" s="22" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D8" s="26">
-        <v>16.5</v>
-      </c>
-      <c r="E8" s="24" t="s">
+    <row r="18" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="O18" s="22">
+        <v>3.6109811718037399</v>
+      </c>
+      <c r="P18" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="O8" s="23">
-        <v>11.964063493612199</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q8" s="23" t="s">
+      <c r="Q18" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="R8" s="23" t="s">
+      <c r="R18" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="T8" s="23">
-        <v>13.5</v>
-      </c>
-      <c r="U8" s="23">
-        <v>2</v>
-      </c>
-      <c r="V8" s="23" t="s">
+      <c r="T18" s="22">
+        <v>4</v>
+      </c>
+      <c r="U18" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="V18" s="22" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D9" s="26">
-        <v>13.1</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="O9" s="23">
-        <v>10.952546728525</v>
-      </c>
-      <c r="P9" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q9" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R9" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T9" s="23">
-        <v>12.3</v>
-      </c>
-      <c r="U9" s="23">
-        <v>2.8</v>
-      </c>
-      <c r="V9" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D10" s="26">
-        <v>12</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="O10" s="23">
-        <v>14.612808547428401</v>
-      </c>
-      <c r="P10" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q10" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R10" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T10" s="23">
-        <v>16.5</v>
-      </c>
-      <c r="U10" s="23">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="V10" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D11" s="26">
-        <v>10.5</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="O11" s="23">
-        <v>16.6551455158944</v>
-      </c>
-      <c r="P11" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q11" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R11" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T11" s="23">
-        <v>14.7</v>
-      </c>
-      <c r="U11" s="23">
-        <v>0.8</v>
-      </c>
-      <c r="V11" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D12" s="26">
-        <v>5.2</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="O12" s="23">
-        <v>12.3101841702579</v>
-      </c>
-      <c r="P12" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q12" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R12" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T12" s="23">
-        <v>13.9</v>
-      </c>
-      <c r="U12" s="23">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="V12" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D13" s="26">
-        <v>4</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="O13" s="23">
-        <v>14.655472173093001</v>
-      </c>
-      <c r="P13" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q13" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R13" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T13" s="23">
-        <v>16.5</v>
-      </c>
-      <c r="U13" s="23">
-        <v>2.6</v>
-      </c>
-      <c r="V13" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O14" s="23">
-        <v>11.7451230687414</v>
-      </c>
-      <c r="P14" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q14" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R14" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T14" s="23">
-        <v>13.1</v>
-      </c>
-      <c r="U14" s="23">
-        <v>1.6</v>
-      </c>
-      <c r="V14" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O15" s="23">
-        <v>10.6283233670864</v>
-      </c>
-      <c r="P15" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q15" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R15" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T15" s="23">
-        <v>12</v>
-      </c>
-      <c r="U15" s="23">
-        <v>2.1</v>
-      </c>
-      <c r="V15" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O16" s="23">
-        <v>9.3685672762428993</v>
-      </c>
-      <c r="P16" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q16" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R16" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T16" s="23">
-        <v>10.5</v>
-      </c>
-      <c r="U16" s="23">
-        <v>1.7</v>
-      </c>
-      <c r="V16" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="15:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O17" s="23">
-        <v>4.6942755233448503</v>
-      </c>
-      <c r="P17" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q17" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R17" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T17" s="23">
-        <v>5.2</v>
-      </c>
-      <c r="U17" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="V17" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="15:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O18" s="23">
-        <v>3.6109811718037399</v>
-      </c>
-      <c r="P18" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q18" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="R18" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="T18" s="23">
-        <v>4</v>
-      </c>
-      <c r="U18" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="V18" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="15:22" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="15:22" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2168,10 +2191,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2229,7 +2252,7 @@
         <v>127</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2252,7 +2275,7 @@
         <v>129</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2367,7 +2390,7 @@
         <v>141</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2390,7 +2413,7 @@
         <v>143</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2619,7 +2642,7 @@
         <v>160</v>
       </c>
       <c r="D21" s="14">
-        <v>480</v>
+        <v>12</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>123</v>
@@ -2632,7 +2655,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="L21" s="3"/>
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2657,21 +2680,21 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="L22" s="3"/>
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>166</v>
+      <c r="A23" s="19" t="s">
+        <v>192</v>
       </c>
       <c r="B23" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="D23" s="16" t="s">
         <v>168</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>169</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>123</v>
@@ -2679,26 +2702,26 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
+      <c r="L23" s="3"/>
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>139</v>
+      <c r="A24" s="19" t="s">
+        <v>166</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>123</v>
@@ -2706,26 +2729,22 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+      <c r="L24" s="3"/>
       <c r="M24" s="2"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>175</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>123</v>
@@ -2733,22 +2752,22 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="18" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
+      <c r="L25" s="3"/>
       <c r="M25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="17" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>123</v>
@@ -2756,12 +2775,12 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
+      <c r="L26" s="3"/>
       <c r="M26" s="2"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -2777,8 +2796,8 @@
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="26"/>
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -2794,8 +2813,8 @@
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="26"/>
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -2811,8 +2830,8 @@
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
       <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -2828,9 +2847,206 @@
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
       <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>